<commit_message>
added rest time comparison and a better way to view slots
</commit_message>
<xml_diff>
--- a/data/9-29-19_data/League-2019-09-29-mod.xlsx
+++ b/data/9-29-19_data/League-2019-09-29-mod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\9-29-19_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F5D19B-FA0A-4C22-963C-A0F2C2AAD9B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3A4974-A51E-4031-8C40-30B7E752813A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="30" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -57,18 +57,12 @@
     <t>CL</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>Major</t>
   </si>
   <si>
     <t>Maj</t>
   </si>
   <si>
-    <t>16</t>
-  </si>
-  <si>
     <t>Minor</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
   </si>
   <si>
     <t>PW</t>
-  </si>
-  <si>
-    <t>14</t>
   </si>
   <si>
     <t>CoachPitch</t>
@@ -451,7 +442,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +470,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -487,22 +478,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
+      <c r="F2">
+        <v>16</v>
       </c>
       <c r="G2">
         <v>120</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -510,22 +501,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
       </c>
       <c r="G3">
         <v>120</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -533,22 +524,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>16</v>
       </c>
       <c r="G4">
         <v>105</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -556,16 +547,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>16</v>
       </c>
       <c r="G5">
         <v>105</v>
@@ -579,16 +570,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
+      <c r="F6">
+        <v>14</v>
       </c>
       <c r="G6">
         <v>90</v>
@@ -602,16 +593,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
-        <v>9</v>
+      <c r="F7">
+        <v>8</v>
       </c>
       <c r="G7">
         <v>60</v>
@@ -633,8 +624,8 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
-        <v>9</v>
+      <c r="F8">
+        <v>8</v>
       </c>
       <c r="G8">
         <v>60</v>

</xml_diff>